<commit_message>
form matching of fromexcel.py working again
</commit_message>
<xml_diff>
--- a/test/data/excel/small_cog.xlsx
+++ b/test/data/excel/small_cog.xlsx
@@ -16,7 +16,7 @@
     <definedName name="pn163olsbqdj">#REF!</definedName>
     <definedName name="y96sxjudtbsk">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -83,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B43" authorId="0">
+    <comment ref="B18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -96,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B49" authorId="0">
+    <comment ref="B20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -109,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B50" authorId="0">
+    <comment ref="B21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
   <si>
     <t>English</t>
   </si>
@@ -186,24 +186,12 @@
     <t>ONE3</t>
   </si>
   <si>
-    <t>ONE4</t>
-  </si>
-  <si>
-    <t>ONE5</t>
-  </si>
-  <si>
     <t>ONE6</t>
   </si>
   <si>
     <t>/etakrã/; /etakɾã/ [e.ta.'kɾã] (uno; solo){4}</t>
   </si>
   <si>
-    <t>ONE7</t>
-  </si>
-  <si>
-    <t>ONE8</t>
-  </si>
-  <si>
     <t>two</t>
   </si>
   <si>
@@ -225,36 +213,6 @@
     <t>[mõˈkõj̃]</t>
   </si>
   <si>
-    <t>TWO2</t>
-  </si>
-  <si>
-    <t>TWO3</t>
-  </si>
-  <si>
-    <t>TWO4</t>
-  </si>
-  <si>
-    <t>TWO5</t>
-  </si>
-  <si>
-    <t>TWO6</t>
-  </si>
-  <si>
-    <t>TWO7</t>
-  </si>
-  <si>
-    <t>TWO8</t>
-  </si>
-  <si>
-    <t>TWO9</t>
-  </si>
-  <si>
-    <t>TWO10</t>
-  </si>
-  <si>
-    <t>TWO11</t>
-  </si>
-  <si>
     <t>three</t>
   </si>
   <si>
@@ -276,24 +234,6 @@
     <t>[mbohaˈpɨ]</t>
   </si>
   <si>
-    <t>THREE2</t>
-  </si>
-  <si>
-    <t>THREE3</t>
-  </si>
-  <si>
-    <t>THREE4</t>
-  </si>
-  <si>
-    <t>THREE5</t>
-  </si>
-  <si>
-    <t>THREE6</t>
-  </si>
-  <si>
-    <t>THREE7</t>
-  </si>
-  <si>
     <t>THREE8</t>
   </si>
   <si>
@@ -327,21 +267,6 @@
     <t>[iɾũndɨ]</t>
   </si>
   <si>
-    <t>FOUR2</t>
-  </si>
-  <si>
-    <t>FOUR3</t>
-  </si>
-  <si>
-    <t>FOUR5</t>
-  </si>
-  <si>
-    <t>FOUR6</t>
-  </si>
-  <si>
-    <t>FOUR7</t>
-  </si>
-  <si>
     <t>FOUR8</t>
   </si>
   <si>
@@ -366,22 +291,10 @@
     <t>FIVE2</t>
   </si>
   <si>
-    <t>FIVE3</t>
-  </si>
-  <si>
-    <t>FIVE4</t>
-  </si>
-  <si>
     <t>FIVE5</t>
   </si>
   <si>
     <t>[teʔiowaa], [teɲoˈʔa]</t>
-  </si>
-  <si>
-    <t>FIVE6</t>
-  </si>
-  <si>
-    <t>FIVE7</t>
   </si>
   <si>
     <t>LOAN</t>
@@ -409,7 +322,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -429,12 +342,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="1"/>
     </font>
@@ -870,13 +777,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1:J2"/>
+      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="12.5"/>
@@ -886,7 +793,7 @@
     <col min="3" max="3" width="6.26953125" customWidth="1"/>
     <col min="4" max="5" width="8.08984375" customWidth="1"/>
     <col min="6" max="6" width="7.08984375" customWidth="1"/>
-    <col min="7" max="10" width="8.08984375" customWidth="1"/>
+    <col min="7" max="10" width="11.54296875" customWidth="1"/>
     <col min="985" max="1024" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -930,16 +837,16 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="6" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="11.25" customHeight="1">
@@ -1023,7 +930,9 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="G7" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -1031,13 +940,19 @@
     <row r="8" spans="1:10" ht="11.25" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="D8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -1045,29 +960,35 @@
     <row r="9" spans="1:10" ht="11.25" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="11.25" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="6"/>
+      <c r="D10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -1075,32 +996,34 @@
     <row r="11" spans="1:10" ht="11.25" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="J11" s="6" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="11.25" customHeight="1">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="4" t="s">
-        <v>28</v>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -1109,31 +1032,33 @@
     <row r="13" spans="1:10" ht="11.25" customHeight="1">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13" s="5"/>
-      <c r="J13" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="G13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" ht="11.25" customHeight="1">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="D14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -1141,27 +1066,35 @@
     <row r="15" spans="1:10" ht="11.25" customHeight="1">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
+      <c r="G15" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="11.25" customHeight="1">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="G16" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
@@ -1169,23 +1102,33 @@
     <row r="17" spans="1:10" ht="11.25" customHeight="1">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C17" s="5"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="D17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I17" s="6"/>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="5"/>
+      <c r="A18" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -1197,7 +1140,7 @@
     <row r="19" spans="1:10" ht="11.25" customHeight="1">
       <c r="A19" s="4"/>
       <c r="B19" s="5" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="4"/>
@@ -1206,14 +1149,18 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="J19" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="20" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="5"/>
+      <c r="A20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="9"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1223,466 +1170,20 @@
       <c r="J20" s="4"/>
     </row>
     <row r="21" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-    </row>
-    <row r="23" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-    </row>
-    <row r="25" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I25" s="5"/>
-      <c r="J25" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-    </row>
-    <row r="27" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-    </row>
-    <row r="28" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-    </row>
-    <row r="29" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-    </row>
-    <row r="31" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-    </row>
-    <row r="32" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="6" t="s">
+      <c r="A21" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-    </row>
-    <row r="33" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A33" s="4"/>
-      <c r="B33" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="6" t="s">
+      <c r="B21" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-    </row>
-    <row r="34" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A34" s="4"/>
-      <c r="B34" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-    </row>
-    <row r="35" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A35" s="4"/>
-      <c r="B35" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I35" s="5"/>
-      <c r="J35" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A36" s="4"/>
-      <c r="B36" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-    </row>
-    <row r="37" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A37" s="4"/>
-      <c r="B37" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-    </row>
-    <row r="38" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A38" s="4"/>
-      <c r="B38" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-    </row>
-    <row r="39" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A39" s="4"/>
-      <c r="B39" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-    </row>
-    <row r="40" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A40" s="4"/>
-      <c r="B40" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-    </row>
-    <row r="41" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A41" s="4"/>
-      <c r="B41" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-    </row>
-    <row r="42" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A42" s="4"/>
-      <c r="B42" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F42" s="5"/>
-      <c r="G42" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="I42" s="6"/>
-      <c r="J42" s="4"/>
-    </row>
-    <row r="43" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A43" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-    </row>
-    <row r="44" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A44" s="4"/>
-      <c r="B44" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-    </row>
-    <row r="45" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A45" s="4"/>
-      <c r="B45" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-    </row>
-    <row r="46" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A46" s="4"/>
-      <c r="B46" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A47" s="4"/>
-      <c r="B47" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-    </row>
-    <row r="48" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A48" s="4"/>
-      <c r="B48" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-    </row>
-    <row r="49" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A49" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-    </row>
-    <row r="50" spans="1:10" ht="11.25" customHeight="1">
-      <c r="A50" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
deleted empty rows in cognate test file
</commit_message>
<xml_diff>
--- a/test/data/excel/small_cog.xlsx
+++ b/test/data/excel/small_cog.xlsx
@@ -783,7 +783,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="12.5"/>
@@ -793,7 +793,8 @@
     <col min="3" max="3" width="6.26953125" customWidth="1"/>
     <col min="4" max="5" width="8.08984375" customWidth="1"/>
     <col min="6" max="6" width="7.08984375" customWidth="1"/>
-    <col min="7" max="10" width="11.54296875" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" customWidth="1"/>
+    <col min="8" max="10" width="11.54296875" customWidth="1"/>
     <col min="985" max="1024" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
slightly modified for debugging matching
</commit_message>
<xml_diff>
--- a/test/data/excel/small_cog.xlsx
+++ b/test/data/excel/small_cog.xlsx
@@ -168,9 +168,6 @@
     <t>ONE1</t>
   </si>
   <si>
-    <t>&lt;peteĩ&gt; #peteĩ#; &lt;peteĩha&gt;#peteĩha# (FIRST)</t>
-  </si>
-  <si>
     <t>[petẽˈʔĩ]</t>
   </si>
   <si>
@@ -316,6 +313,9 @@
   </si>
   <si>
     <t>ECC/ZJO: DONE S/L</t>
+  </si>
+  <si>
+    <t>&lt;peteĩ&gt; ; &lt;peteĩha&gt; (FIRST)</t>
   </si>
 </sst>
 </file>
@@ -783,7 +783,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1:G1048576"/>
+      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="12.5"/>
@@ -838,16 +838,16 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="11.25" customHeight="1">
@@ -879,19 +879,19 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="5" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="11.25" customHeight="1">
       <c r="A5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="4"/>
@@ -899,19 +899,19 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="11.25" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="4"/>
@@ -925,14 +925,14 @@
     <row r="7" spans="1:10" ht="11.25" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -941,18 +941,18 @@
     <row r="8" spans="1:10" ht="11.25" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -961,7 +961,7 @@
     <row r="9" spans="1:10" ht="11.25" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="4"/>
@@ -969,24 +969,24 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="11.25" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="4"/>
@@ -997,34 +997,34 @@
     <row r="11" spans="1:10" ht="11.25" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="11.25" customHeight="1">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -1033,14 +1033,14 @@
     <row r="13" spans="1:10" ht="11.25" customHeight="1">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -1049,14 +1049,14 @@
     <row r="14" spans="1:10" ht="11.25" customHeight="1">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="6"/>
@@ -1067,34 +1067,34 @@
     <row r="15" spans="1:10" ht="11.25" customHeight="1">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="11.25" customHeight="1">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -1103,31 +1103,31 @@
     <row r="17" spans="1:10" ht="11.25" customHeight="1">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" ht="11.25" customHeight="1">
       <c r="A18" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>53</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
@@ -1141,7 +1141,7 @@
     <row r="19" spans="1:10" ht="11.25" customHeight="1">
       <c r="A19" s="4"/>
       <c r="B19" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="4"/>
@@ -1151,15 +1151,15 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="11.25" customHeight="1">
       <c r="A20" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>57</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="4"/>
@@ -1172,10 +1172,10 @@
     </row>
     <row r="21" spans="1:10" ht="11.25" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="11"/>

</xml_diff>

<commit_message>
deleted some ## in the cells
</commit_message>
<xml_diff>
--- a/test/data/excel/small_cog.xlsx
+++ b/test/data/excel/small_cog.xlsx
@@ -177,9 +177,6 @@
     <t>ONE2</t>
   </si>
   <si>
-    <t>&lt;peteĩ&gt; #peteĩ#</t>
-  </si>
-  <si>
     <t>ONE3</t>
   </si>
   <si>
@@ -204,9 +201,6 @@
     <t>TWO1</t>
   </si>
   <si>
-    <t>&lt;mokõi&gt; #mokõi#</t>
-  </si>
-  <si>
     <t>[mõˈkõj̃]</t>
   </si>
   <si>
@@ -225,9 +219,6 @@
     <t>/buǰa1/</t>
   </si>
   <si>
-    <t>&lt;mbohapy&gt; #mbohapɨ#</t>
-  </si>
-  <si>
     <t>[mbohaˈpɨ]</t>
   </si>
   <si>
@@ -316,6 +307,15 @@
   </si>
   <si>
     <t>&lt;peteĩ&gt; ; &lt;peteĩha&gt; (FIRST)</t>
+  </si>
+  <si>
+    <t>&lt;peteĩ&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mokõi&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mbohapy&gt;</t>
   </si>
 </sst>
 </file>
@@ -783,7 +783,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomRight" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="12.5"/>
@@ -838,16 +838,16 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="11.25" customHeight="1">
@@ -879,7 +879,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="6" t="s">
@@ -899,7 +899,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="5" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="6" t="s">
@@ -911,7 +911,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="4"/>
@@ -925,14 +925,14 @@
     <row r="7" spans="1:10" ht="11.25" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -941,18 +941,18 @@
     <row r="8" spans="1:10" ht="11.25" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -961,7 +961,7 @@
     <row r="9" spans="1:10" ht="11.25" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="4"/>
@@ -969,24 +969,24 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="5" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="11.25" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="4"/>
@@ -997,34 +997,34 @@
     <row r="11" spans="1:10" ht="11.25" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="11.25" customHeight="1">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -1033,14 +1033,14 @@
     <row r="13" spans="1:10" ht="11.25" customHeight="1">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -1049,14 +1049,14 @@
     <row r="14" spans="1:10" ht="11.25" customHeight="1">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="6"/>
@@ -1067,34 +1067,34 @@
     <row r="15" spans="1:10" ht="11.25" customHeight="1">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="11.25" customHeight="1">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -1103,31 +1103,31 @@
     <row r="17" spans="1:10" ht="11.25" customHeight="1">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" ht="11.25" customHeight="1">
       <c r="A18" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
@@ -1141,7 +1141,7 @@
     <row r="19" spans="1:10" ht="11.25" customHeight="1">
       <c r="A19" s="4"/>
       <c r="B19" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="4"/>
@@ -1151,15 +1151,15 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="11.25" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="4"/>
@@ -1172,10 +1172,10 @@
     </row>
     <row r="21" spans="1:10" ht="11.25" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="11"/>

</xml_diff>